<commit_message>
Remove unused author information
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/authors.xlsx
+++ b/chiloPro/template-series/authors.xlsx
@@ -5,15 +5,14 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer_pri\chiloPro\template-series\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="日置慎治" sheetId="10" r:id="rId1"/>
-    <sheet name="Template" sheetId="7" r:id="rId2"/>
+    <sheet name="Template" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>picture</t>
     <phoneticPr fontId="1"/>
@@ -124,52 +123,6 @@
     <rPh sb="167" eb="169">
       <t>キサイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>001_photo.png</t>
-  </si>
-  <si>
-    <t>HIOKI, Shinji</t>
-  </si>
-  <si>
-    <t>帝塚山大学経営学部教授</t>
-  </si>
-  <si>
-    <t>博士（工学）</t>
-  </si>
-  <si>
-    <t>学位</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>大阪大学基礎工学研究科数理専攻博士後期課程修了。工学博士。 広島大学理学部助手等を経て、現在、帝塚山大学経営学部教授、学部長。ゴードン・ベル賞受賞（1995）</t>
-  </si>
-  <si>
-    <t>物理学 / 素粒子・原子核・宇宙線・宇宙物理 / 情報学 / 図書館情報学・人文社会情報学</t>
-  </si>
-  <si>
-    <t>シミュレーション(292) , 格子QCD(4) , 数値シミュレ-ション(94) , ハドロン(12) , 並列計算(50) , 有限温度質量(1) , 質量移行(1) , ハイパフォ-マンス(1) , ハイパフォ-マンスコンピュ-ティング(20) , ス-パ-コンピュ-タ(11) , 有限温度(2) , クオ-ク・グル-ホン・プラズマ(1) , 質量(6) , トポロジ-(44) , 格子色力学(QCD)(1) , モンテカルロシミュレ-ション(25) , 人口(29) , グルーオン(5) , インターネット(219) , 江戸時代(19)</t>
-  </si>
-  <si>
-    <t>【専門分野】</t>
-    <rPh sb="1" eb="3">
-      <t>センモン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ブンヤ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>【研究キーワード】</t>
-    <rPh sb="1" eb="3">
-      <t>ケンキュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日置 慎治</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -227,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,12 +190,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,7 +359,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -430,9 +377,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -827,123 +771,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
-    <col min="2" max="2" width="50.625" customWidth="1"/>
-    <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C4:D8"/>
-  </mergeCells>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -955,72 +782,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
close #37 Set the default image of the author to the series directory template
</commit_message>
<xml_diff>
--- a/chiloPro/template-series/authors.xlsx
+++ b/chiloPro/template-series/authors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>picture</t>
     <phoneticPr fontId="1"/>
@@ -123,6 +123,10 @@
     <rPh sb="167" eb="169">
       <t>キサイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>template_photo.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -785,7 +789,9 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C1" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>